<commit_message>
Fixed loss of data when there were spaces in column names.
</commit_message>
<xml_diff>
--- a/Data/Priest River/soilChem_y5/KEY_PREF_y5_soilChemEPP.xlsx
+++ b/Data/Priest River/soilChem_y5/KEY_PREF_y5_soilChemEPP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\EDaH\Data\Priest River\soilChem_y5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E7A172-FC2D-4D75-8C3D-9A5656570667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE51AEE-6EAC-4C08-BE12-B77BDDB1DF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3855" yWindow="3900" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2125" uniqueCount="725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2124" uniqueCount="725">
   <si>
     <t>var</t>
   </si>
@@ -2717,7 +2717,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C32" sqref="C32"/>
+      <selection pane="topRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4048,9 +4048,6 @@
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="14">
         <v>83.8</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>42</v>

</xml_diff>